<commit_message>
Optimized code for faster execution: - Compiled user code only once per submission file to reduce redundancy - Reduced redundant file I/O operations by reusing data across tests - Streamlined Excel report generation with single question list retrieval - Enhanced subprocess handling to avoid repeated calls
</commit_message>
<xml_diff>
--- a/Darshan/Results/test_results.xlsx
+++ b/Darshan/Results/test_results.xlsx
@@ -429,17 +429,17 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Ques3</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>Ques1</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Ques2</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Ques3</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -456,17 +456,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -481,21 +481,21 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>33.3%</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>66.7%</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>33.3%</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>5.333333333333333</v>
       </c>
     </row>
     <row r="4">
@@ -506,17 +506,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="E4" t="n">

</xml_diff>

<commit_message>
Updated code to support individual marks per question: - Replaced uniform marks with per-question-specific marks in evaluation and reporting - Adjusted report generation logic to reflect varying question marks
</commit_message>
<xml_diff>
--- a/Darshan/Results/test_results.xlsx
+++ b/Darshan/Results/test_results.xlsx
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -495,7 +495,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>5.333333333333333</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Added support for Java
- Added compile and run functions for Java.
- Automatically detect and handle both C++ and Java submissions.
- Optimized runtime with separate functions for language-specific operations.
</commit_message>
<xml_diff>
--- a/Darshan/Results/test_results.xlsx
+++ b/Darshan/Results/test_results.xlsx
@@ -429,17 +429,17 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Ques1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Ques2</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>Ques3</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Ques1</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Ques2</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -469,8 +469,10 @@
           <t>100.0%</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>22</v>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>12.0</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -481,21 +483,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>66.7%</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>33.3%</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>66.7%</t>
-        </is>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>33.3%</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>9</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>5.7</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -516,11 +520,13 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved failed test case display and fastend the code removing redundancy reads.
</commit_message>
<xml_diff>
--- a/Darshan/Results/test_results.xlsx
+++ b/Darshan/Results/test_results.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>66.7%</t>
+          <t>33.3%</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -498,7 +498,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>4.0</t>
         </is>
       </c>
     </row>
@@ -510,14 +510,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>33.3%</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>0.0%</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>100.0%</t>
@@ -525,7 +525,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>5.7</t>
         </is>
       </c>
     </row>

</xml_diff>